<commit_message>
Addition of another test
</commit_message>
<xml_diff>
--- a/test-analysis/WebTestHackathon.xlsx
+++ b/test-analysis/WebTestHackathon.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="86">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -190,6 +190,12 @@
     <t>Message "Invalid code ..!"</t>
   </si>
   <si>
+    <t>Click Add to Cart on a different item without increasing its quantity</t>
+  </si>
+  <si>
+    <t>The price should be 1xprice of the item i added but its not - Defect ID 1</t>
+  </si>
+  <si>
     <t>Defect ID</t>
   </si>
   <si>
@@ -208,13 +214,13 @@
     <t>Defect detailed Description</t>
   </si>
   <si>
-    <t>The amount of money is not calculated correctly when the user has changed the quantity of another item and then trying to add to the cart a different one</t>
+    <t>The amount of money is not calculated correctly when the user has changed the quantity of a specific item and then trying to add to the cart a different one</t>
   </si>
   <si>
     <t>Complementary Information</t>
   </si>
   <si>
-    <t>The multiplier of the cost of an item seems to be the quantity of the item we changed before,without adding it to the cart</t>
+    <t>The multiplier of the cost of an added item seems to be the quantity of the item we last updated before,without adding it to the cart. Then, the multiplier truly resets</t>
   </si>
   <si>
     <t>Label name misspelling</t>
@@ -232,10 +238,10 @@
     <t>The order begins shipping when the user's country was not selected.</t>
   </si>
   <si>
-    <t>The amount of money is not calculated correctly when the user has changed the quantity of another item and then instantly trying to add to the cart a different one</t>
-  </si>
-  <si>
-    <t>The multiplier of the cost of an item seems to be the quantity of the item we changed before, for a specific time period,for a specific time period, without adding it to the cart</t>
+    <t>The amount of money is not calculated correctly when the user has changed the quantity of a specific item and then instantly trying to add to the cart a different one</t>
+  </si>
+  <si>
+    <t>The multiplier of the cost of an added item seems to be the quantity of the item we updated before,for a specific small time period, without adding it to the cart</t>
   </si>
   <si>
     <t xml:space="preserve">Delivery date in the past </t>
@@ -1588,6 +1594,14 @@
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="6"/>
+      <c r="G55" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H55" s="4">
+        <v>12.0</v>
+      </c>
+      <c r="I55" s="5"/>
+      <c r="J55" s="6"/>
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
@@ -1598,6 +1612,14 @@
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="10"/>
+      <c r="G56" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I56" s="9"/>
+      <c r="J56" s="10"/>
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
@@ -1608,6 +1630,14 @@
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="6"/>
+      <c r="G57" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="5"/>
+      <c r="J57" s="6"/>
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
@@ -1618,6 +1648,14 @@
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
+      <c r="G58" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I58" s="5"/>
+      <c r="J58" s="6"/>
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
@@ -1630,6 +1668,16 @@
       <c r="D59" s="13" t="s">
         <v>9</v>
       </c>
+      <c r="G59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59" s="7"/>
+      <c r="J59" s="13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="14">
@@ -1642,6 +1690,16 @@
       <c r="D60" s="7" t="s">
         <v>56</v>
       </c>
+      <c r="G60" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I60" s="15"/>
+      <c r="J60" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="7">
@@ -1654,10 +1712,20 @@
       <c r="D61" s="7" t="s">
         <v>58</v>
       </c>
+      <c r="G61" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I61" s="15"/>
+      <c r="J61" s="18" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B65" s="26">
         <v>1.0</v>
@@ -1671,10 +1739,10 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -1699,10 +1767,10 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -1713,10 +1781,10 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -1727,10 +1795,10 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
@@ -1756,7 +1824,7 @@
     </row>
     <row r="73">
       <c r="A73" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B73" s="26">
         <v>2.0</v>
@@ -1770,10 +1838,10 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -1796,10 +1864,10 @@
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -1810,10 +1878,10 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -1824,7 +1892,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B78" s="20"/>
       <c r="C78" s="9"/>
@@ -1846,7 +1914,7 @@
     </row>
     <row r="81">
       <c r="A81" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B81" s="26">
         <v>3.0</v>
@@ -1860,10 +1928,10 @@
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
@@ -1888,10 +1956,10 @@
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -1902,10 +1970,10 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -1916,7 +1984,7 @@
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B86" s="20"/>
       <c r="C86" s="9"/>
@@ -1928,7 +1996,7 @@
     </row>
     <row r="89">
       <c r="A89" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B89" s="26">
         <v>4.0</v>
@@ -1942,10 +2010,10 @@
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -1970,10 +2038,10 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -1984,10 +2052,10 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -1998,10 +2066,10 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B94" s="20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
@@ -2012,7 +2080,7 @@
     </row>
     <row r="97">
       <c r="A97" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B97" s="26">
         <v>5.0</v>
@@ -2026,10 +2094,10 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -2054,10 +2122,10 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -2068,10 +2136,10 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -2082,7 +2150,7 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B102" s="20"/>
       <c r="C102" s="9"/>
@@ -2094,7 +2162,7 @@
     </row>
     <row r="105">
       <c r="A105" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B105" s="26">
         <v>6.0</v>
@@ -2108,10 +2176,10 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -2134,10 +2202,10 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -2148,10 +2216,10 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -2162,7 +2230,7 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B110" s="20"/>
       <c r="C110" s="9"/>
@@ -2177,16 +2245,16 @@
         <v>0</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C114" s="28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D114" s="27" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E114" s="27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="115">
@@ -2246,7 +2314,7 @@
       <c r="E122" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="84">
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="H36:J36"/>
@@ -2322,11 +2390,15 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="H57:J57"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="H44:J44"/>
     <mergeCell ref="H45:J45"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="H47:J47"/>
+    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="H55:J55"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>